<commit_message>
Add Excel with first-pass of new metabolism genes
</commit_message>
<xml_diff>
--- a/notebooks/new_environments/new_genes.xlsx
+++ b/notebooks/new_environments/new_genes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timjing/Documents/vivarium-ecoli/notebooks/new_environments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA23580A-CCC1-0940-BCEA-CA0625D586C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14043F5-703F-3E4E-BAA4-A762C314C0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,16 +23,12 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={233A7065-C82E-9047-AECB-4BB2C60C0ED7}</author>
-    <author>tc={A1D62331-6CBD-464B-A7C0-6A5B944B272F}</author>
     <author>tc={CAD60B6D-7CA4-EB41-8146-89DC21BBF0A1}</author>
     <author>tc={85DF0CB5-8598-8446-A378-A39C54F01DA0}</author>
     <author>tc={2ACF1440-B38B-F44C-9870-EE6EF4544B58}</author>
     <author>tc={E8A14C1E-5320-DB40-9ED4-23A4C04AF5B9}</author>
     <author>Microsoft Office User</author>
     <author>tc={7313F797-670B-3547-BF19-1C0632F5B49F}</author>
-    <author>tc={6FA941BA-1E8F-DE46-AF66-885307048C32}</author>
-    <author>tc={F104B7FF-3838-2744-AAD1-74D5A4AE8400}</author>
-    <author>tc={155B0B3E-8CAC-C64B-89EF-E72CD6700781}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{233A7065-C82E-9047-AECB-4BB2C60C0ED7}">
@@ -43,15 +39,7 @@
     No slashes in name</t>
       </text>
     </comment>
-    <comment ref="A9" authorId="1" shapeId="0" xr:uid="{A1D62331-6CBD-464B-A7C0-6A5B944B272F}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Transport still not being used</t>
-      </text>
-    </comment>
-    <comment ref="A12" authorId="2" shapeId="0" xr:uid="{CAD60B6D-7CA4-EB41-8146-89DC21BBF0A1}">
+    <comment ref="A12" authorId="1" shapeId="0" xr:uid="{CAD60B6D-7CA4-EB41-8146-89DC21BBF0A1}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -59,7 +47,7 @@
     Cellobiose Pathway Explored Only</t>
       </text>
     </comment>
-    <comment ref="A14" authorId="3" shapeId="0" xr:uid="{85DF0CB5-8598-8446-A378-A39C54F01DA0}">
+    <comment ref="A14" authorId="2" shapeId="0" xr:uid="{85DF0CB5-8598-8446-A378-A39C54F01DA0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -67,7 +55,7 @@
     CPD-20903 (COBIIALAMIN) is not added since only the [c] form is available</t>
       </text>
     </comment>
-    <comment ref="E14" authorId="4" shapeId="0" xr:uid="{2ACF1440-B38B-F44C-9870-EE6EF4544B58}">
+    <comment ref="E14" authorId="3" shapeId="0" xr:uid="{2ACF1440-B38B-F44C-9870-EE6EF4544B58}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -75,7 +63,7 @@
     Demand necessary to generate flux</t>
       </text>
     </comment>
-    <comment ref="A52" authorId="5" shapeId="0" xr:uid="{E8A14C1E-5320-DB40-9ED4-23A4C04AF5B9}">
+    <comment ref="A52" authorId="4" shapeId="0" xr:uid="{E8A14C1E-5320-DB40-9ED4-23A4C04AF5B9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -83,7 +71,7 @@
     Special reaction currently has no flux. It does assist with the fructose pts transport, which does have flux</t>
       </text>
     </comment>
-    <comment ref="B52" authorId="6" shapeId="0" xr:uid="{942EDE5F-D682-CE48-861F-D56050281344}">
+    <comment ref="B52" authorId="5" shapeId="0" xr:uid="{942EDE5F-D682-CE48-861F-D56050281344}">
       <text>
         <r>
           <rPr>
@@ -107,7 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B60" authorId="6" shapeId="0" xr:uid="{0DE697B8-2938-D447-AE12-B98C57F48A85}">
+    <comment ref="B60" authorId="5" shapeId="0" xr:uid="{0DE697B8-2938-D447-AE12-B98C57F48A85}">
       <text>
         <r>
           <rPr>
@@ -131,7 +119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A64" authorId="7" shapeId="0" xr:uid="{7313F797-670B-3547-BF19-1C0632F5B49F}">
+    <comment ref="A64" authorId="6" shapeId="0" xr:uid="{7313F797-670B-3547-BF19-1C0632F5B49F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -139,60 +127,12 @@
     Maybe issue with having general classes of molecules</t>
       </text>
     </comment>
-    <comment ref="B67" authorId="6" shapeId="0" xr:uid="{4889393F-C039-AE40-AE8F-F422D692A8B3}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Microsoft Office User:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A74" authorId="8" shapeId="0" xr:uid="{6FA941BA-1E8F-DE46-AF66-885307048C32}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Issue with general compounds?</t>
-      </text>
-    </comment>
-    <comment ref="A76" authorId="9" shapeId="0" xr:uid="{F104B7FF-3838-2744-AAD1-74D5A4AE8400}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    CPD-20903 (COBIIALAMIN) is not added since only the [c] form is available</t>
-      </text>
-    </comment>
-    <comment ref="E76" authorId="10" shapeId="0" xr:uid="{155B0B3E-8CAC-C64B-89EF-E72CD6700781}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Demand necessary to generate flux</t>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="212">
   <si>
     <t>Environment</t>
   </si>
@@ -284,6 +224,12 @@
     <t>7-AMINOMETHYL-7-DEAZAGUANINE[c]</t>
   </si>
   <si>
+    <t>Acetate Transport</t>
+  </si>
+  <si>
+    <t>EG11942</t>
+  </si>
+  <si>
     <t>Substrates</t>
   </si>
   <si>
@@ -431,6 +377,9 @@
     <t>EG12522, EG12760</t>
   </si>
   <si>
+    <t>D-GALACTARATE[p], PROTON[p]</t>
+  </si>
+  <si>
     <t>EG20080</t>
   </si>
   <si>
@@ -819,106 +768,13 @@
   </si>
   <si>
     <t>Ascorbate + vit C PTS Transport + Catabolism</t>
-  </si>
-  <si>
-    <t>D-GALACTARATE[p]</t>
-  </si>
-  <si>
-    <t>EG11942, EG10023, EG10022</t>
-  </si>
-  <si>
-    <t>Acetate Transport + Metabolism</t>
-  </si>
-  <si>
-    <t>Periplasmic Phosphatase to Import G6P</t>
-  </si>
-  <si>
-    <t>EG10033</t>
-  </si>
-  <si>
-    <t>GLC-1-P[p]</t>
-  </si>
-  <si>
-    <t>Cell Wall Component Biosynthesis</t>
-  </si>
-  <si>
-    <t>EG11788</t>
-  </si>
-  <si>
-    <t>CPD-13118[c]</t>
-  </si>
-  <si>
-    <t>Galactose Deg, Cell Envelope Biosynth</t>
-  </si>
-  <si>
-    <t>EG11319</t>
-  </si>
-  <si>
-    <t>GALACTOSE[p]</t>
-  </si>
-  <si>
-    <t>MALTOSE[p]</t>
-  </si>
-  <si>
-    <t>EG10528</t>
-  </si>
-  <si>
-    <t>Outer Membrane Generic Ion+Sugar Transport, Lambda Receptor</t>
-  </si>
-  <si>
-    <t>GLU[p]</t>
-  </si>
-  <si>
-    <t>EG11055, EG11658</t>
-  </si>
-  <si>
-    <t>gluconoride transport + gluconoride and gluconorate catabolism</t>
-  </si>
-  <si>
-    <t>TRIMETHYLAMINE-N-O[p]</t>
-  </si>
-  <si>
-    <t>EG11814, EG11815, G7022</t>
-  </si>
-  <si>
-    <t>anaerobic growth using TMAO as acceptor</t>
-  </si>
-  <si>
-    <t>ARG[p]</t>
-  </si>
-  <si>
-    <t>EG10959</t>
-  </si>
-  <si>
-    <t>putrescine (ubiquitious regulator) biosynthesis</t>
-  </si>
-  <si>
-    <t>N-acetyl-D-glucosamine[p]</t>
-  </si>
-  <si>
-    <t>EG10633, EG10635</t>
-  </si>
-  <si>
-    <t>N-acetylglucosamine degradation I</t>
-  </si>
-  <si>
-    <t>L-SELENOCYSTEINE[c]</t>
-  </si>
-  <si>
-    <t>SEPO3[c], SER[c]</t>
-  </si>
-  <si>
-    <t>EG10941</t>
-  </si>
-  <si>
-    <t>Testing L-Selenocysteine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -984,12 +840,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1038,7 +888,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1060,8 +910,6 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1375,9 +1223,6 @@
   <threadedComment ref="A1" dT="2023-06-29T18:18:51.61" personId="{637DA067-3816-7541-B31D-1CFBEB7BD9A2}" id="{233A7065-C82E-9047-AECB-4BB2C60C0ED7}">
     <text>No slashes in name</text>
   </threadedComment>
-  <threadedComment ref="A9" dT="2023-06-30T22:26:11.99" personId="{637DA067-3816-7541-B31D-1CFBEB7BD9A2}" id="{A1D62331-6CBD-464B-A7C0-6A5B944B272F}">
-    <text>Transport still not being used</text>
-  </threadedComment>
   <threadedComment ref="A12" dT="2023-06-28T00:41:57.84" personId="{637DA067-3816-7541-B31D-1CFBEB7BD9A2}" id="{CAD60B6D-7CA4-EB41-8146-89DC21BBF0A1}">
     <text>Cellobiose Pathway Explored Only</text>
   </threadedComment>
@@ -1393,24 +1238,15 @@
   <threadedComment ref="A64" dT="2023-06-28T23:27:18.81" personId="{637DA067-3816-7541-B31D-1CFBEB7BD9A2}" id="{7313F797-670B-3547-BF19-1C0632F5B49F}">
     <text>Maybe issue with having general classes of molecules</text>
   </threadedComment>
-  <threadedComment ref="A74" dT="2023-07-10T17:11:48.00" personId="{637DA067-3816-7541-B31D-1CFBEB7BD9A2}" id="{6FA941BA-1E8F-DE46-AF66-885307048C32}">
-    <text>Issue with general compounds?</text>
-  </threadedComment>
-  <threadedComment ref="A76" dT="2023-06-28T00:57:04.82" personId="{637DA067-3816-7541-B31D-1CFBEB7BD9A2}" id="{F104B7FF-3838-2744-AAD1-74D5A4AE8400}">
-    <text>CPD-20903 (COBIIALAMIN) is not added since only the [c] form is available</text>
-  </threadedComment>
-  <threadedComment ref="E76" dT="2023-06-28T01:00:53.45" personId="{637DA067-3816-7541-B31D-1CFBEB7BD9A2}" id="{155B0B3E-8CAC-C64B-89EF-E72CD6700781}">
-    <text>Demand necessary to generate flux</text>
-  </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1445,7 +1281,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1550,7 +1386,7 @@
     </row>
     <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>28</v>
@@ -1564,31 +1400,29 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>211</v>
+      <c r="A9" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>210</v>
+        <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1597,16 +1431,16 @@
     </row>
     <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -1614,13 +1448,13 @@
     </row>
     <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>17</v>
@@ -1631,13 +1465,13 @@
     </row>
     <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>17</v>
@@ -1648,30 +1482,30 @@
     </row>
     <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>17</v>
@@ -1682,13 +1516,13 @@
     </row>
     <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>17</v>
@@ -1699,13 +1533,13 @@
     </row>
     <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>22</v>
@@ -1716,13 +1550,13 @@
     </row>
     <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1731,13 +1565,13 @@
     </row>
     <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1746,13 +1580,13 @@
     </row>
     <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1761,13 +1595,13 @@
     </row>
     <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>17</v>
@@ -1778,13 +1612,13 @@
     </row>
     <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>17</v>
@@ -1795,13 +1629,13 @@
     </row>
     <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1810,13 +1644,13 @@
     </row>
     <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>17</v>
@@ -1827,13 +1661,13 @@
     </row>
     <row r="25" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>17</v>
@@ -1844,45 +1678,43 @@
     </row>
     <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>181</v>
-      </c>
-      <c r="B27" t="s">
-        <v>78</v>
-      </c>
-      <c r="C27" t="s">
-        <v>209</v>
-      </c>
-      <c r="D27" t="s">
-        <v>17</v>
-      </c>
+    <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1891,13 +1723,13 @@
     </row>
     <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1906,28 +1738,28 @@
     </row>
     <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D30"/>
+        <v>88</v>
+      </c>
+      <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1936,13 +1768,13 @@
     </row>
     <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>17</v>
@@ -1953,13 +1785,13 @@
     </row>
     <row r="33" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>17</v>
@@ -1970,10 +1802,10 @@
     </row>
     <row r="34" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>13</v>
@@ -1987,10 +1819,10 @@
     </row>
     <row r="35" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>13</v>
@@ -2004,13 +1836,13 @@
     </row>
     <row r="36" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -2019,47 +1851,47 @@
     </row>
     <row r="37" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
     </row>
     <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
     </row>
     <row r="39" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>17</v>
@@ -2070,13 +1902,13 @@
     </row>
     <row r="40" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>17</v>
@@ -2087,13 +1919,13 @@
     </row>
     <row r="41" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>17</v>
@@ -2104,13 +1936,13 @@
     </row>
     <row r="42" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>17</v>
@@ -2121,13 +1953,13 @@
     </row>
     <row r="43" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>17</v>
@@ -2138,13 +1970,13 @@
     </row>
     <row r="44" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -2153,13 +1985,13 @@
     </row>
     <row r="45" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -2168,16 +2000,16 @@
     </row>
     <row r="46" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
@@ -2185,13 +2017,13 @@
     </row>
     <row r="47" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -2200,13 +2032,13 @@
     </row>
     <row r="48" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -2215,30 +2047,30 @@
     </row>
     <row r="49" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
     </row>
     <row r="50" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -2247,13 +2079,13 @@
     </row>
     <row r="51" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -2262,13 +2094,13 @@
     </row>
     <row r="52" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>17</v>
@@ -2279,32 +2111,32 @@
     </row>
     <row r="53" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
     </row>
     <row r="54" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -2313,13 +2145,13 @@
     </row>
     <row r="55" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -2328,30 +2160,30 @@
     </row>
     <row r="56" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
     </row>
     <row r="57" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>17</v>
@@ -2362,13 +2194,13 @@
     </row>
     <row r="58" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>22</v>
@@ -2379,13 +2211,13 @@
     </row>
     <row r="59" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>17</v>
@@ -2396,13 +2228,13 @@
     </row>
     <row r="60" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -2411,30 +2243,30 @@
     </row>
     <row r="61" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -2443,13 +2275,13 @@
     </row>
     <row r="63" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>17</v>
@@ -2460,13 +2292,13 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -2475,13 +2307,13 @@
     </row>
     <row r="65" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>17</v>
@@ -2492,143 +2324,18 @@
     </row>
     <row r="66" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
-    </row>
-    <row r="67" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A67" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="D67" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D68" s="2"/>
-    </row>
-    <row r="69" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A69" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B69" s="9" t="s">
-        <v>219</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A70" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="B70" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A71" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="B71" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A72" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="B72" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A73" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A74" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A76" s="2"/>
-      <c r="B76" s="3"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
-      <c r="E76" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Update Excel with first-pass of second set of metabolism genes
</commit_message>
<xml_diff>
--- a/notebooks/new_environments/new_genes.xlsx
+++ b/notebooks/new_environments/new_genes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timjing/Documents/vivarium-ecoli/notebooks/new_environments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14043F5-703F-3E4E-BAA4-A762C314C0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD73870-921A-074F-818C-E93E74EEE509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,12 +23,14 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={233A7065-C82E-9047-AECB-4BB2C60C0ED7}</author>
+    <author>tc={A1D62331-6CBD-464B-A7C0-6A5B944B272F}</author>
     <author>tc={CAD60B6D-7CA4-EB41-8146-89DC21BBF0A1}</author>
     <author>tc={85DF0CB5-8598-8446-A378-A39C54F01DA0}</author>
     <author>tc={2ACF1440-B38B-F44C-9870-EE6EF4544B58}</author>
     <author>tc={E8A14C1E-5320-DB40-9ED4-23A4C04AF5B9}</author>
     <author>Microsoft Office User</author>
     <author>tc={7313F797-670B-3547-BF19-1C0632F5B49F}</author>
+    <author>tc={6FA941BA-1E8F-DE46-AF66-885307048C32}</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{233A7065-C82E-9047-AECB-4BB2C60C0ED7}">
@@ -39,7 +41,15 @@
     No slashes in name</t>
       </text>
     </comment>
-    <comment ref="A12" authorId="1" shapeId="0" xr:uid="{CAD60B6D-7CA4-EB41-8146-89DC21BBF0A1}">
+    <comment ref="A9" authorId="1" shapeId="0" xr:uid="{A1D62331-6CBD-464B-A7C0-6A5B944B272F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Transport still not being used</t>
+      </text>
+    </comment>
+    <comment ref="A12" authorId="2" shapeId="0" xr:uid="{CAD60B6D-7CA4-EB41-8146-89DC21BBF0A1}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -47,7 +57,7 @@
     Cellobiose Pathway Explored Only</t>
       </text>
     </comment>
-    <comment ref="A14" authorId="2" shapeId="0" xr:uid="{85DF0CB5-8598-8446-A378-A39C54F01DA0}">
+    <comment ref="A14" authorId="3" shapeId="0" xr:uid="{85DF0CB5-8598-8446-A378-A39C54F01DA0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -55,7 +65,7 @@
     CPD-20903 (COBIIALAMIN) is not added since only the [c] form is available</t>
       </text>
     </comment>
-    <comment ref="E14" authorId="3" shapeId="0" xr:uid="{2ACF1440-B38B-F44C-9870-EE6EF4544B58}">
+    <comment ref="E14" authorId="4" shapeId="0" xr:uid="{2ACF1440-B38B-F44C-9870-EE6EF4544B58}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -63,7 +73,7 @@
     Demand necessary to generate flux</t>
       </text>
     </comment>
-    <comment ref="A52" authorId="4" shapeId="0" xr:uid="{E8A14C1E-5320-DB40-9ED4-23A4C04AF5B9}">
+    <comment ref="A52" authorId="5" shapeId="0" xr:uid="{E8A14C1E-5320-DB40-9ED4-23A4C04AF5B9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -71,7 +81,7 @@
     Special reaction currently has no flux. It does assist with the fructose pts transport, which does have flux</t>
       </text>
     </comment>
-    <comment ref="B52" authorId="5" shapeId="0" xr:uid="{942EDE5F-D682-CE48-861F-D56050281344}">
+    <comment ref="B52" authorId="6" shapeId="0" xr:uid="{942EDE5F-D682-CE48-861F-D56050281344}">
       <text>
         <r>
           <rPr>
@@ -95,7 +105,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B60" authorId="5" shapeId="0" xr:uid="{0DE697B8-2938-D447-AE12-B98C57F48A85}">
+    <comment ref="B60" authorId="6" shapeId="0" xr:uid="{0DE697B8-2938-D447-AE12-B98C57F48A85}">
       <text>
         <r>
           <rPr>
@@ -119,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A64" authorId="6" shapeId="0" xr:uid="{7313F797-670B-3547-BF19-1C0632F5B49F}">
+    <comment ref="A64" authorId="7" shapeId="0" xr:uid="{7313F797-670B-3547-BF19-1C0632F5B49F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -127,12 +137,44 @@
     Maybe issue with having general classes of molecules</t>
       </text>
     </comment>
+    <comment ref="B67" authorId="6" shapeId="0" xr:uid="{4889393F-C039-AE40-AE8F-F422D692A8B3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A74" authorId="8" shapeId="0" xr:uid="{6FA941BA-1E8F-DE46-AF66-885307048C32}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Issue with general compounds?</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="236">
   <si>
     <t>Environment</t>
   </si>
@@ -224,12 +266,6 @@
     <t>7-AMINOMETHYL-7-DEAZAGUANINE[c]</t>
   </si>
   <si>
-    <t>Acetate Transport</t>
-  </si>
-  <si>
-    <t>EG11942</t>
-  </si>
-  <si>
     <t>Substrates</t>
   </si>
   <si>
@@ -377,9 +413,6 @@
     <t>EG12522, EG12760</t>
   </si>
   <si>
-    <t>D-GALACTARATE[p], PROTON[p]</t>
-  </si>
-  <si>
     <t>EG20080</t>
   </si>
   <si>
@@ -768,13 +801,94 @@
   </si>
   <si>
     <t>Ascorbate + vit C PTS Transport + Catabolism</t>
+  </si>
+  <si>
+    <t>D-GALACTARATE[p]</t>
+  </si>
+  <si>
+    <t>EG11942, EG10023, EG10022</t>
+  </si>
+  <si>
+    <t>Acetate Transport + Metabolism</t>
+  </si>
+  <si>
+    <t>Periplasmic Phosphatase to Import G6P</t>
+  </si>
+  <si>
+    <t>EG10033</t>
+  </si>
+  <si>
+    <t>GLC-1-P[p]</t>
+  </si>
+  <si>
+    <t>Cell Wall Component Biosynthesis</t>
+  </si>
+  <si>
+    <t>EG11788</t>
+  </si>
+  <si>
+    <t>CPD-13118[c]</t>
+  </si>
+  <si>
+    <t>Galactose Deg, Cell Envelope Biosynth</t>
+  </si>
+  <si>
+    <t>EG11319</t>
+  </si>
+  <si>
+    <t>GALACTOSE[p]</t>
+  </si>
+  <si>
+    <t>MALTOSE[p]</t>
+  </si>
+  <si>
+    <t>EG10528</t>
+  </si>
+  <si>
+    <t>Outer Membrane Generic Ion+Sugar Transport, Lambda Receptor</t>
+  </si>
+  <si>
+    <t>GLU[p]</t>
+  </si>
+  <si>
+    <t>EG11055, EG11658</t>
+  </si>
+  <si>
+    <t>gluconoride transport + gluconoride and gluconorate catabolism</t>
+  </si>
+  <si>
+    <t>TRIMETHYLAMINE-N-O[p]</t>
+  </si>
+  <si>
+    <t>EG11814, EG11815, G7022</t>
+  </si>
+  <si>
+    <t>anaerobic growth using TMAO as acceptor</t>
+  </si>
+  <si>
+    <t>ARG[p]</t>
+  </si>
+  <si>
+    <t>EG10959</t>
+  </si>
+  <si>
+    <t>putrescine (ubiquitious regulator) biosynthesis</t>
+  </si>
+  <si>
+    <t>N-acetyl-D-glucosamine[p]</t>
+  </si>
+  <si>
+    <t>EG10633, EG10635</t>
+  </si>
+  <si>
+    <t>N-acetylglucosamine degradation I</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -840,6 +954,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -888,7 +1008,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -910,6 +1030,8 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1223,6 +1345,9 @@
   <threadedComment ref="A1" dT="2023-06-29T18:18:51.61" personId="{637DA067-3816-7541-B31D-1CFBEB7BD9A2}" id="{233A7065-C82E-9047-AECB-4BB2C60C0ED7}">
     <text>No slashes in name</text>
   </threadedComment>
+  <threadedComment ref="A9" dT="2023-06-30T22:26:11.99" personId="{637DA067-3816-7541-B31D-1CFBEB7BD9A2}" id="{A1D62331-6CBD-464B-A7C0-6A5B944B272F}">
+    <text>Transport still not being used</text>
+  </threadedComment>
   <threadedComment ref="A12" dT="2023-06-28T00:41:57.84" personId="{637DA067-3816-7541-B31D-1CFBEB7BD9A2}" id="{CAD60B6D-7CA4-EB41-8146-89DC21BBF0A1}">
     <text>Cellobiose Pathway Explored Only</text>
   </threadedComment>
@@ -1238,15 +1363,18 @@
   <threadedComment ref="A64" dT="2023-06-28T23:27:18.81" personId="{637DA067-3816-7541-B31D-1CFBEB7BD9A2}" id="{7313F797-670B-3547-BF19-1C0632F5B49F}">
     <text>Maybe issue with having general classes of molecules</text>
   </threadedComment>
+  <threadedComment ref="A74" dT="2023-07-10T17:11:48.00" personId="{637DA067-3816-7541-B31D-1CFBEB7BD9A2}" id="{6FA941BA-1E8F-DE46-AF66-885307048C32}">
+    <text>Issue with general compounds?</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G66"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1281,7 +1409,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1386,7 +1514,7 @@
     </row>
     <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>28</v>
@@ -1400,29 +1528,31 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>30</v>
+      <c r="A9" t="s">
+        <v>211</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>31</v>
+        <v>210</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1431,16 +1561,16 @@
     </row>
     <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -1448,13 +1578,13 @@
     </row>
     <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>17</v>
@@ -1465,13 +1595,13 @@
     </row>
     <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>17</v>
@@ -1482,30 +1612,30 @@
     </row>
     <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>17</v>
@@ -1516,13 +1646,13 @@
     </row>
     <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>17</v>
@@ -1533,13 +1663,13 @@
     </row>
     <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>22</v>
@@ -1550,13 +1680,13 @@
     </row>
     <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1565,13 +1695,13 @@
     </row>
     <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1580,13 +1710,13 @@
     </row>
     <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1595,13 +1725,13 @@
     </row>
     <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>17</v>
@@ -1612,13 +1742,13 @@
     </row>
     <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>17</v>
@@ -1629,13 +1759,13 @@
     </row>
     <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1644,13 +1774,13 @@
     </row>
     <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>17</v>
@@ -1661,13 +1791,13 @@
     </row>
     <row r="25" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>17</v>
@@ -1678,43 +1808,45 @@
     </row>
     <row r="26" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D27" s="2"/>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>181</v>
+      </c>
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" t="s">
+        <v>209</v>
+      </c>
+      <c r="D27" t="s">
+        <v>17</v>
+      </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1723,13 +1855,13 @@
     </row>
     <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1738,28 +1870,28 @@
     </row>
     <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D30" s="2"/>
+        <v>85</v>
+      </c>
+      <c r="D30"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1768,13 +1900,13 @@
     </row>
     <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>17</v>
@@ -1785,13 +1917,13 @@
     </row>
     <row r="33" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>17</v>
@@ -1802,10 +1934,10 @@
     </row>
     <row r="34" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>13</v>
@@ -1819,10 +1951,10 @@
     </row>
     <row r="35" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>13</v>
@@ -1836,13 +1968,13 @@
     </row>
     <row r="36" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -1851,47 +1983,47 @@
     </row>
     <row r="37" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
     </row>
     <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
     </row>
     <row r="39" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>17</v>
@@ -1902,13 +2034,13 @@
     </row>
     <row r="40" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>17</v>
@@ -1919,13 +2051,13 @@
     </row>
     <row r="41" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>17</v>
@@ -1936,13 +2068,13 @@
     </row>
     <row r="42" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>17</v>
@@ -1953,13 +2085,13 @@
     </row>
     <row r="43" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>17</v>
@@ -1970,13 +2102,13 @@
     </row>
     <row r="44" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -1985,13 +2117,13 @@
     </row>
     <row r="45" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -2000,16 +2132,16 @@
     </row>
     <row r="46" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
@@ -2017,13 +2149,13 @@
     </row>
     <row r="47" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -2032,13 +2164,13 @@
     </row>
     <row r="48" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
@@ -2047,30 +2179,30 @@
     </row>
     <row r="49" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
     </row>
     <row r="50" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -2079,13 +2211,13 @@
     </row>
     <row r="51" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
@@ -2094,13 +2226,13 @@
     </row>
     <row r="52" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>17</v>
@@ -2111,32 +2243,32 @@
     </row>
     <row r="53" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
     </row>
     <row r="54" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -2145,13 +2277,13 @@
     </row>
     <row r="55" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -2160,30 +2292,30 @@
     </row>
     <row r="56" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
     </row>
     <row r="57" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>17</v>
@@ -2194,13 +2326,13 @@
     </row>
     <row r="58" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>22</v>
@@ -2211,13 +2343,13 @@
     </row>
     <row r="59" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>17</v>
@@ -2228,13 +2360,13 @@
     </row>
     <row r="60" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -2243,30 +2375,30 @@
     </row>
     <row r="61" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -2275,13 +2407,13 @@
     </row>
     <row r="63" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>17</v>
@@ -2292,13 +2424,13 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -2307,13 +2439,13 @@
     </row>
     <row r="65" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>17</v>
@@ -2324,18 +2456,122 @@
     </row>
     <row r="66" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
+    </row>
+    <row r="67" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A67" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D67" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A68" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A70" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A71" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A72" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="B72" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A73" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A74" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>224</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fixed homeostatic value estimate based on reactions where the demand compound is the reactant
</commit_message>
<xml_diff>
--- a/notebooks/new_environments/new_genes.xlsx
+++ b/notebooks/new_environments/new_genes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timjing/Documents/vivarium-ecoli/notebooks/new_environments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD73870-921A-074F-818C-E93E74EEE509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81515ED-554B-4E4F-BE3D-E100A061E919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1373,8 +1373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>